<commit_message>
Implementation of programNameDefinition and programEntryDefinition
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/User defined words.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="229">
   <si>
     <t>Literal/Symbol</t>
   </si>
@@ -533,9 +533,6 @@
   <si>
     <t>character code set
 collating sequence</t>
-  </si>
-  <si>
-    <t>Leaf rule</t>
   </si>
   <si>
     <t>Def. Rule</t>
@@ -680,12 +677,91 @@
   <si>
     <t>literal</t>
   </si>
+  <si>
+    <t>Original Leaf rule</t>
+  </si>
+  <si>
+    <t>New Leaf rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> programNameDefinition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> programEntryDefinition</t>
+  </si>
+  <si>
+    <t>data
+identifier</t>
+  </si>
+  <si>
+    <t>=fileName with IsRecord=true</t>
+  </si>
+  <si>
+    <t>functionName // values : ACOS, ANNUITY, ASIN, ATAN, CHAR, COS, CURRENT-DATE, DATE-OF-INTEGER, DATE-TO-YYYYMMDD, DAY-OF-INTEGER, DAY-TO-YYYYDDD, DISPLAY-OF, FACTORIAL, INTEGER, INTEGER-OF-DATE, INTEGER-OF-DAY, INTEGER-PART, LENGTH, LOG, LOG10, LOWER-CASE, MAX, MEAN, MEDIAN, MIDRANGE, MIN, MOD, NATIONAL-OF, NUMVAL, NUMVAL-C, ORD, ORD-MAX, ORD-MIN, PRESENT-VALUE, RANDOM, RANGE, REM, REVERSE, SIN, SQRT, STANDARD-DEVIATION, SUM, TAN, ULENGTH, UPOS, UPPER-CASE, USUBSTR, USUPPLEMENTARY, UVALID, UWIDTH, VARIANCE, WHEN-COMPILED, YEAR-TO-YYYY</t>
+  </si>
+  <si>
+    <t>lit.enum : functionIdentifier</t>
+  </si>
+  <si>
+    <t>=textName</t>
+  </si>
+  <si>
+    <t>=assignmentName</t>
+  </si>
+  <si>
+    <t>// Runtime functions</t>
+  </si>
+  <si>
+    <t>[FunctionName]</t>
+  </si>
+  <si>
+    <t>[Keywords]</t>
+  </si>
+  <si>
+    <t>[ExecTranslatorName]</t>
+  </si>
+  <si>
+    <t>[SymbolicCharacter]</t>
+  </si>
+  <si>
+    <t>lit.enum : execStatement</t>
+  </si>
+  <si>
+    <t>ExecTranslatorName</t>
+  </si>
+  <si>
+    <t>specialRegister</t>
+  </si>
+  <si>
+    <t>lit.enum : dataNameReferenceOrSpecialRegisterOrFunctionIdentifier</t>
+  </si>
+  <si>
+    <t>ref : figurativeConstant (alphanumericLiteralBase)</t>
+  </si>
+  <si>
+    <t>def : symbolicCharactersOrdinalPositions (symbolicCharactersClause / specialNamesParagraph)</t>
+  </si>
+  <si>
+    <t>programNameReference2</t>
+  </si>
+  <si>
+    <t>programNameReference1
+programNameFromData</t>
+  </si>
+  <si>
+    <t>programNameReferenceOrProgramEntryReference
+programNameFromDataOrProgramEntryFromDataOrProcedurePointerOrFunctionPointer</t>
+  </si>
+  <si>
+    <t>programNameReferenceOrProgramEntryReference
+programNameFromDataOrProgramEntryFromData</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,6 +778,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -733,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -755,6 +852,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,466 +1353,541 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>70</v>
+      <c r="A47" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>71</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>72</v>
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>100</v>
+      <c r="C84" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>101</v>
+      <c r="C85" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>119</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
+      <c r="B127" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+      <c r="B131" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>145</v>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>148</v>
+      <c r="A147" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B150" t="s">
-        <v>150</v>
+      <c r="B149" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B152" t="s">
+    <row r="170" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="171" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
+    <row r="172" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B172" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="173" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
+    <row r="174" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="175" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="10" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
+    <row r="176" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="10" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,17 +1899,18 @@
     <col min="5" max="5" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="88.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="47.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="54" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="4"/>
+    <col min="8" max="8" width="30.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="88.5703125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="47.85546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="54" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1742,34 +1927,37 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1786,31 +1974,34 @@
         <v>38</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>176</v>
+      <c r="H2" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="M2" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1818,37 +2009,40 @@
         <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="L3" s="7" t="s">
+      <c r="H3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1862,16 +2056,16 @@
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1885,16 +2079,16 @@
         <v>21</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1911,13 +2105,13 @@
         <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1931,16 +2125,16 @@
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1951,13 +2145,13 @@
         <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1968,13 +2162,13 @@
         <v>20</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1988,7 +2182,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1996,7 +2190,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -2004,7 +2198,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -2012,7 +2206,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -2020,7 +2214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -2031,7 +2225,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -2220,10 +2414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,144 +2426,160 @@
     <col min="2" max="2" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="131.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="32" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="131.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>176</v>
+      <c r="E5" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -2377,7 +2587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -2385,7 +2595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -2395,7 +2605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -2403,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -2411,7 +2621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Section names and pargraph names OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/User defined words.xlsx
+++ b/TypeCobol/Documentation/Studies/User defined words.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\TypeCobol\TypeCobol\Documentation\Studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/196f0b5afced95ca/Dev/Github/TypeCobol/TypeCobol/Documentation/Studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12240" tabRatio="607" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="247">
   <si>
     <t>Literal/Symbol</t>
   </si>
@@ -559,19 +559,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>Ambiguity at def.</t>
-  </si>
-  <si>
     <t>Ref. code elt</t>
   </si>
   <si>
     <t>Ref. Rule</t>
-  </si>
-  <si>
-    <t>Ambiguity at ref.</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Restrictions</t>
@@ -631,19 +622,11 @@
 literal</t>
   </si>
   <si>
-    <t>identifier (USAGE DISPLAY)
-procedurePointer (dataName USAGE IS PROCEDURE-POINTER)
-functionPointer (dataName USAGE IS FUNCTION-POINTER)</t>
-  </si>
-  <si>
     <t>identifierOrLiteral</t>
   </si>
   <si>
     <t>identifier-1 must be an alphanumeric, alphabetic, or zoned decimal data item such that its value can be a program-name.
 literal-1 or the contents of identifier-1 must be the same as a literal or the contents of an identifier specified in an associated CALL statement.</t>
-  </si>
-  <si>
-    <t>No (ENTRY keyword is unique)</t>
   </si>
   <si>
     <t>identifier-8 : Must be defined as an alphabetic or alphanumeric item such that the value can be a program name
@@ -690,10 +673,6 @@
     <t xml:space="preserve"> programEntryDefinition</t>
   </si>
   <si>
-    <t>data
-identifier</t>
-  </si>
-  <si>
     <t>=fileName with IsRecord=true</t>
   </si>
   <si>
@@ -755,13 +734,103 @@
   <si>
     <t>programNameReferenceOrProgramEntryReference
 programNameFromDataOrProgramEntryFromData</t>
+  </si>
+  <si>
+    <t>sectionNameDefinition</t>
+  </si>
+  <si>
+    <t>paragraphNameDefinition</t>
+  </si>
+  <si>
+    <t>A referenced section-name, because it cannot be qualified, must be unique within the program in which it is defined.</t>
+  </si>
+  <si>
+    <t>A user-defined word</t>
+  </si>
+  <si>
+    <t>Paragraphs need not all be contained within sections</t>
+  </si>
+  <si>
+    <t>A paragraph-name, because it can be qualified, need not be unique.</t>
+  </si>
+  <si>
+    <t>sortStatement</t>
+  </si>
+  <si>
+    <t>xmlParseStatement</t>
+  </si>
+  <si>
+    <t>useStatementForDebuggingDeclarative</t>
+  </si>
+  <si>
+    <t>gotoStatement</t>
+  </si>
+  <si>
+    <t>performProcedureStatement</t>
+  </si>
+  <si>
+    <t>alterStatement</t>
+  </si>
+  <si>
+    <t>procedureName</t>
+  </si>
+  <si>
+    <t>SectionName
+ParagraphName</t>
+  </si>
+  <si>
+    <t>ProgramName
+ProgramEntry</t>
+  </si>
+  <si>
+    <t>ProgramName
+ProgrameEntry</t>
+  </si>
+  <si>
+    <t>paragraphNameOrSectionNameReference
+qualifiedParagraphNameReference
+   &gt; paragraphNameReference
+   &gt; sectionNameReference</t>
+  </si>
+  <si>
+    <t>Must name a procedure or a section in the same PROCEDURE DIVISION as the GO TO statement.</t>
+  </si>
+  <si>
+    <t>Must name a section or paragraph in the procedure division.
+When both procedure-name-1 and procedure-name-2 are specified, if either is a procedure-name in a declarative procedure, both must be procedure-names in the same declarative procedure. The only necessary relationship between procedure-name-1 and procedure-name-2 is that a consecutive sequence of operations is executed, beginning at the procedure named by procedure-name-1 and ending with the execution of the procedure named by procedure-name-2.</t>
+  </si>
+  <si>
+    <t>inputStatement
+outputStament</t>
+  </si>
+  <si>
+    <t>procedure-name-1 : Specifies the first (or only) section or paragraph in the input procedure.
+procedure-name-2 : Identifies the last section or paragraph of the input procedure.</t>
+  </si>
+  <si>
+    <t>Must not be defined in a debugging session.
+Any given procedure-name can appear in only one USE FOR DEBUGGING sentence, and only once in that sentence. 
+All procedures must appear in the outermost program.</t>
+  </si>
+  <si>
+    <t>Within the PROCEDURE DIVISION, a procedure consists of a section or a group of sections, and a paragraph or group of paragraphs.
+A procedure-name is a user-defined name that identifies a section or a paragraph.
+procedure-name-1 : Must name a PROCEDURE DIVISION paragraph that contains only one sentence: a GO TO statement without the DEPENDING ON phrase. 
+procedure-name-2 : Must name a PROCEDURE DIVISION section or paragraph.</t>
+  </si>
+  <si>
+    <t>Must name a section or paragraph in the PROCEDURE DIVISION.
+When both procedure-name-1 and procedure-name-2 are specified, if either is a procedure name in a declarative procedure, both must be procedure names in the same declarative procedure.
+procedure-name-1 : Specifies the first (or only) section or paragraph in the processing procedure.
+procedure-name-2 : Specifies the last section or paragraph in the processing procedure.
+The only necessary relationship between procedure-name-1 and procedure-name-2 is that they define a consecutive sequence of operations to execute, beginning at the procedure named by procedure-name-1 and ending with the execution of the procedure named by procedure-name-2.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,6 +872,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -830,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -865,6 +941,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,18 +1294,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1247,43 +1324,43 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1354,17 +1431,17 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1569,17 +1646,17 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -1632,7 +1709,7 @@
         <v>119</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -1680,7 +1757,7 @@
         <v>127</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -1703,7 +1780,7 @@
         <v>131</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -1738,37 +1815,37 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,10 +1961,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7605" ySplit="600" topLeftCell="K4" activePane="bottomRight"/>
+      <selection activeCell="G3" sqref="G3"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,14 +1984,13 @@
     <col min="9" max="9" width="6.140625" style="5" customWidth="1"/>
     <col min="10" max="10" width="5.7109375" style="5" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="88.5703125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="47.85546875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="54" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="4"/>
+    <col min="12" max="12" width="88.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="47.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="54" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1930,10 +2010,10 @@
         <v>168</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>31</v>
@@ -1945,19 +2025,16 @@
         <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1980,7 +2057,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>175</v>
@@ -1988,20 +2065,17 @@
       <c r="J2" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>180</v>
+      <c r="L2" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -2009,40 +2083,37 @@
         <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>180</v>
+      <c r="L3" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2064,8 +2135,20 @@
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -2087,8 +2170,23 @@
       <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2111,7 +2209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2134,7 +2232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -2151,7 +2249,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -2168,7 +2266,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -2182,7 +2280,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -2190,7 +2288,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -2198,7 +2296,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -2206,7 +2304,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -2214,7 +2312,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -2225,7 +2323,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -2414,42 +2512,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5160" ySplit="600" topLeftCell="D1" activePane="bottomRight"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="131.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="4"/>
+    <col min="9" max="9" width="131.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>31</v>
@@ -2461,113 +2562,98 @@
         <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>181</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>238</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>169</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>208</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="F2" s="8"/>
       <c r="G2" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>169</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>208</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="F3" s="8"/>
       <c r="G3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>22</v>
+      <c r="I3" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>208</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="F4" s="8"/>
       <c r="G4" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I4" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>175</v>
@@ -2575,58 +2661,138 @@
       <c r="G5" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
+    </row>
+    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>235</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+        <v>235</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>235</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>64</v>
+        <v>235</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>